<commit_message>
mse for mc done
</commit_message>
<xml_diff>
--- a/04_files/HUDM6026 final project.xlsx
+++ b/04_files/HUDM6026 final project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panpeter/Desktop/PhD_Learning/HUDM6026 Computational Statistics/HUDM6026_Final_Project/04_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC339437-6EF4-7F4B-81F2-AD08B8B4C23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B52EA8A-B237-B14F-AED0-017D7BB3735A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="29940" windowHeight="18740" xr2:uid="{E5AD6347-145B-EC4A-AF39-F259BCD8375F}"/>
+    <workbookView xWindow="4360" yWindow="6140" windowWidth="29940" windowHeight="18740" xr2:uid="{E5AD6347-145B-EC4A-AF39-F259BCD8375F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>